<commit_message>
Birthday update in page and excel
</commit_message>
<xml_diff>
--- a/src/main/resources/testData/patientData.xlsx
+++ b/src/main/resources/testData/patientData.xlsx
@@ -70,7 +70,7 @@
     <t>Female</t>
   </si>
   <si>
-    <t>August 17 2003</t>
+    <t>August/17/2003</t>
   </si>
   <si>
     <t xml:space="preserve">510 Carolann Walk     </t>
@@ -100,7 +100,7 @@
     <t>Schumm</t>
   </si>
   <si>
-    <t>November 22 1989</t>
+    <t>November/22/1989</t>
   </si>
   <si>
     <t xml:space="preserve">1304 Zaida Prairie    </t>
@@ -136,7 +136,7 @@
     <t>Male</t>
   </si>
   <si>
-    <t>January 15 1994</t>
+    <t>June/27/1943</t>
   </si>
   <si>
     <t xml:space="preserve">87484 Torp Mews       </t>
@@ -169,7 +169,7 @@
     <t>Nikolaus</t>
   </si>
   <si>
-    <t>December 07 1991</t>
+    <t>December/07/1991</t>
   </si>
   <si>
     <t xml:space="preserve">8698 Schaden Creek    </t>
@@ -199,7 +199,7 @@
     <t>Roob</t>
   </si>
   <si>
-    <t>January 22 1961</t>
+    <t>January/22/1961</t>
   </si>
   <si>
     <t xml:space="preserve">951 Rafael Branch     </t>
@@ -226,7 +226,7 @@
     <t>Beahan</t>
   </si>
   <si>
-    <t>August 31 1971</t>
+    <t>August/31/1971</t>
   </si>
   <si>
     <t>66993 Alberta Junction</t>
@@ -250,7 +250,7 @@
     <t>Roberts</t>
   </si>
   <si>
-    <t>February 02 1957</t>
+    <t>February/02/1957</t>
   </si>
   <si>
     <t xml:space="preserve">13717 Von Passage     </t>
@@ -277,7 +277,7 @@
     <t>Jacobson</t>
   </si>
   <si>
-    <t>November 22 1957</t>
+    <t>November/22/1957</t>
   </si>
   <si>
     <t>4367 Florencio Prairie</t>
@@ -307,7 +307,7 @@
     <t>Reichel</t>
   </si>
   <si>
-    <t>December 29 1970</t>
+    <t>December/29/1970</t>
   </si>
   <si>
     <t xml:space="preserve">087 Barney Ridges     </t>
@@ -334,7 +334,7 @@
     <t>Gottlieb</t>
   </si>
   <si>
-    <t>January 03 1988</t>
+    <t>January/03/1988</t>
   </si>
   <si>
     <t xml:space="preserve">313 Cremin Drives     </t>
@@ -367,7 +367,7 @@
     <t>Runte</t>
   </si>
   <si>
-    <t>January 20 1986</t>
+    <t>January/20/1986</t>
   </si>
   <si>
     <t xml:space="preserve">637 Marquardt Valley  </t>
@@ -391,7 +391,7 @@
     <t>Turcotte</t>
   </si>
   <si>
-    <t>June 04 1971</t>
+    <t>June/04/1971</t>
   </si>
   <si>
     <t xml:space="preserve">349 Darcy Roads       </t>
@@ -415,7 +415,7 @@
     <t>Willms</t>
   </si>
   <si>
-    <t>March 17 1994</t>
+    <t>March/17/1994</t>
   </si>
   <si>
     <t xml:space="preserve">4872 Gleichner View   </t>
@@ -439,7 +439,7 @@
     <t>Cummings</t>
   </si>
   <si>
-    <t>April 28 1988</t>
+    <t>April/28/1988</t>
   </si>
   <si>
     <t xml:space="preserve">890 Hermann Crossing  </t>
@@ -463,7 +463,7 @@
     <t>O'Keefe</t>
   </si>
   <si>
-    <t>August 31 1979</t>
+    <t>August/31/1979</t>
   </si>
   <si>
     <t xml:space="preserve">32867 Hackett Manors  </t>
@@ -484,7 +484,7 @@
     <t>Reynolds</t>
   </si>
   <si>
-    <t>December 08 1972</t>
+    <t>December/08/1972</t>
   </si>
   <si>
     <t xml:space="preserve">2618 Hank Forge       </t>
@@ -511,7 +511,7 @@
     <t>Weimann</t>
   </si>
   <si>
-    <t>December 10 1935</t>
+    <t>December/10/1935</t>
   </si>
   <si>
     <t xml:space="preserve">8371 Fay Hollow       </t>
@@ -538,7 +538,7 @@
     <t>Hodkiewicz</t>
   </si>
   <si>
-    <t>November 03 1948</t>
+    <t>November/03/1948</t>
   </si>
   <si>
     <t xml:space="preserve">085 Selena Crescent   </t>
@@ -562,7 +562,7 @@
     <t>Kutch</t>
   </si>
   <si>
-    <t>June 27 1926</t>
+    <t>June/27/1926</t>
   </si>
   <si>
     <t xml:space="preserve">665 Devorah Port      </t>
@@ -583,7 +583,7 @@
     <t>Schiller</t>
   </si>
   <si>
-    <t>Jully 26 1960</t>
+    <t>Jully/26/1960</t>
   </si>
   <si>
     <t xml:space="preserve">390 Gretta Hollow     </t>
@@ -610,7 +610,7 @@
     <t>Morissette</t>
   </si>
   <si>
-    <t>Jully 08 1937</t>
+    <t>Jully/08/1937</t>
   </si>
   <si>
     <t xml:space="preserve">60674 Maxima Islands  </t>
@@ -634,7 +634,7 @@
     <t>Lebsack</t>
   </si>
   <si>
-    <t>January 25 1963</t>
+    <t>January/25/1963</t>
   </si>
   <si>
     <t xml:space="preserve">5877 McCullough Track </t>
@@ -655,7 +655,7 @@
     <t>Reinger</t>
   </si>
   <si>
-    <t>September 29 1974</t>
+    <t>September/29/1974</t>
   </si>
   <si>
     <t xml:space="preserve">0074 Kessler Rest     </t>
@@ -673,7 +673,7 @@
     <t>White</t>
   </si>
   <si>
-    <t>January 26 1962</t>
+    <t>January/26/1962</t>
   </si>
   <si>
     <t xml:space="preserve">234 Robel Rue         </t>
@@ -694,7 +694,7 @@
     <t>Nolan</t>
   </si>
   <si>
-    <t>Jully 10 1950</t>
+    <t>Jully/10/1950</t>
   </si>
   <si>
     <t xml:space="preserve">870 Somer Place       </t>
@@ -718,7 +718,7 @@
     <t>Walter</t>
   </si>
   <si>
-    <t>April 23 1969</t>
+    <t>April/23/1969</t>
   </si>
   <si>
     <t xml:space="preserve">13198 Philip Main     </t>
@@ -742,7 +742,7 @@
     <t>MacGyver</t>
   </si>
   <si>
-    <t>December 12 1978</t>
+    <t>December/12/1978</t>
   </si>
   <si>
     <t xml:space="preserve">9544 Yundt Spurs      </t>
@@ -760,7 +760,7 @@
     <t>Konopelski</t>
   </si>
   <si>
-    <t>June 25 1972</t>
+    <t>June/25/1972</t>
   </si>
   <si>
     <t xml:space="preserve">26011 Van Motorway    </t>
@@ -790,7 +790,7 @@
     <t>Bechtelar</t>
   </si>
   <si>
-    <t>September 16 1998</t>
+    <t>September/16/1998</t>
   </si>
   <si>
     <t xml:space="preserve">9733 Emard Lakes      </t>
@@ -813,10 +813,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -834,8 +834,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -843,6 +844,21 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -857,6 +873,14 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -865,31 +889,8 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -903,10 +904,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -917,9 +927,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -938,45 +977,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -984,6 +984,120 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -993,37 +1107,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1035,37 +1149,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1077,97 +1167,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1178,21 +1178,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1216,6 +1201,47 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1246,182 +1272,156 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1762,7 +1762,7 @@
     <sheetView tabSelected="1" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="P8" sqref="P8"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1770,7 +1770,7 @@
     <col min="1" max="1" width="14.9375" customWidth="1"/>
     <col min="2" max="3" width="18.171875" customWidth="1"/>
     <col min="4" max="4" width="13.8125" customWidth="1"/>
-    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="5" max="5" width="22" customWidth="1"/>
     <col min="6" max="6" width="23.375" customWidth="1"/>
     <col min="7" max="7" width="9.3125" customWidth="1"/>
     <col min="8" max="8" width="18.5625" customWidth="1"/>

</xml_diff>

<commit_message>
Login Page is done
</commit_message>
<xml_diff>
--- a/src/main/resources/testData/patientData.xlsx
+++ b/src/main/resources/testData/patientData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28000" windowHeight="11660"/>
+    <workbookView windowWidth="28800" windowHeight="13440"/>
   </bookViews>
   <sheets>
     <sheet name="patientDB" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332">
   <si>
     <t>givenName</t>
   </si>
@@ -64,6 +64,27 @@
     <t>personName</t>
   </si>
   <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>monthNumbers</t>
+  </si>
+  <si>
+    <t>formattedBD</t>
+  </si>
+  <si>
+    <t>currentAge</t>
+  </si>
+  <si>
+    <t>monthNum</t>
+  </si>
+  <si>
     <t>Yuonne</t>
   </si>
   <si>
@@ -97,6 +118,9 @@
     <t>USA</t>
   </si>
   <si>
+    <t>19958</t>
+  </si>
+  <si>
     <t>+2524558455</t>
   </si>
   <si>
@@ -106,6 +130,12 @@
     <t>Vesta</t>
   </si>
   <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
     <t>Shenna</t>
   </si>
   <si>
@@ -133,6 +163,9 @@
     <t>TR</t>
   </si>
   <si>
+    <t>48193</t>
+  </si>
+  <si>
     <t>+2524558456</t>
   </si>
   <si>
@@ -142,6 +175,12 @@
     <t>Carlene</t>
   </si>
   <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>February</t>
+  </si>
+  <si>
     <t>Mittie</t>
   </si>
   <si>
@@ -169,6 +208,9 @@
     <t>RS</t>
   </si>
   <si>
+    <t>96884</t>
+  </si>
+  <si>
     <t>+2524558457</t>
   </si>
   <si>
@@ -178,6 +220,12 @@
     <t>Gavin</t>
   </si>
   <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
     <t>Roland</t>
   </si>
   <si>
@@ -199,6 +247,9 @@
     <t>FR</t>
   </si>
   <si>
+    <t>57037</t>
+  </si>
+  <si>
     <t>+2524558458</t>
   </si>
   <si>
@@ -208,6 +259,12 @@
     <t>Dean</t>
   </si>
   <si>
+    <t>December</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
     <t>Randal</t>
   </si>
   <si>
@@ -232,12 +289,18 @@
     <t>CAN</t>
   </si>
   <si>
+    <t>68925</t>
+  </si>
+  <si>
     <t>+2524558459</t>
   </si>
   <si>
     <t>Michele</t>
   </si>
   <si>
+    <t>May</t>
+  </si>
+  <si>
     <t>Gretchen</t>
   </si>
   <si>
@@ -262,6 +325,9 @@
     <t>GER</t>
   </si>
   <si>
+    <t>88589</t>
+  </si>
+  <si>
     <t>+2524558460</t>
   </si>
   <si>
@@ -289,12 +355,18 @@
     <t>OR</t>
   </si>
   <si>
+    <t>78519</t>
+  </si>
+  <si>
     <t>+2524558461</t>
   </si>
   <si>
     <t>Magdalena</t>
   </si>
   <si>
+    <t>july</t>
+  </si>
+  <si>
     <t>Jonathon</t>
   </si>
   <si>
@@ -316,6 +388,9 @@
     <t>MO</t>
   </si>
   <si>
+    <t>30295</t>
+  </si>
+  <si>
     <t>+2524558462</t>
   </si>
   <si>
@@ -346,6 +421,9 @@
     <t>AL</t>
   </si>
   <si>
+    <t>62931</t>
+  </si>
+  <si>
     <t>+2524558463</t>
   </si>
   <si>
@@ -355,6 +433,9 @@
     <t>Mckinley</t>
   </si>
   <si>
+    <t>September</t>
+  </si>
+  <si>
     <t>Teddy</t>
   </si>
   <si>
@@ -379,6 +460,9 @@
     <t>AZ</t>
   </si>
   <si>
+    <t>39324</t>
+  </si>
+  <si>
     <t>+2524558464</t>
   </si>
   <si>
@@ -388,6 +472,9 @@
     <t>Dionne</t>
   </si>
   <si>
+    <t>October</t>
+  </si>
+  <si>
     <t>Mana</t>
   </si>
   <si>
@@ -409,6 +496,9 @@
     <t>Adalinebury</t>
   </si>
   <si>
+    <t>18672</t>
+  </si>
+  <si>
     <t>+2524558465</t>
   </si>
   <si>
@@ -433,6 +523,9 @@
     <t>NY</t>
   </si>
   <si>
+    <t>82473</t>
+  </si>
+  <si>
     <t>+2524558466</t>
   </si>
   <si>
@@ -457,6 +550,9 @@
     <t>SC</t>
   </si>
   <si>
+    <t>42626</t>
+  </si>
+  <si>
     <t>+2524558467</t>
   </si>
   <si>
@@ -484,6 +580,9 @@
     <t>ME</t>
   </si>
   <si>
+    <t>93077</t>
+  </si>
+  <si>
     <t>+2524558468</t>
   </si>
   <si>
@@ -508,6 +607,9 @@
     <t>Wehnerberg</t>
   </si>
   <si>
+    <t>16820</t>
+  </si>
+  <si>
     <t>+2524558469</t>
   </si>
   <si>
@@ -535,6 +637,9 @@
     <t>NJ</t>
   </si>
   <si>
+    <t>32831</t>
+  </si>
+  <si>
     <t>+2524558470</t>
   </si>
   <si>
@@ -565,6 +670,9 @@
     <t>MD</t>
   </si>
   <si>
+    <t>18661</t>
+  </si>
+  <si>
     <t>+2524558471</t>
   </si>
   <si>
@@ -589,6 +697,9 @@
     <t>KY</t>
   </si>
   <si>
+    <t>57502</t>
+  </si>
+  <si>
     <t>+2524558472</t>
   </si>
   <si>
@@ -613,6 +724,9 @@
     <t>NewSena</t>
   </si>
   <si>
+    <t>44872</t>
+  </si>
+  <si>
     <t>+2524558473</t>
   </si>
   <si>
@@ -622,7 +736,7 @@
     <t>Clay</t>
   </si>
   <si>
-    <t>Jully/26/1960</t>
+    <t>July/26/1960</t>
   </si>
   <si>
     <t>390 Gretta Hollow</t>
@@ -637,6 +751,9 @@
     <t>UT</t>
   </si>
   <si>
+    <t>81932</t>
+  </si>
+  <si>
     <t>+2524558474</t>
   </si>
   <si>
@@ -652,7 +769,7 @@
     <t>Morissette</t>
   </si>
   <si>
-    <t>Jully/08/1937</t>
+    <t>July/08/1937</t>
   </si>
   <si>
     <t>60674 Maxima Islands</t>
@@ -664,6 +781,9 @@
     <t>Florburgh</t>
   </si>
   <si>
+    <t>77790</t>
+  </si>
+  <si>
     <t>+2524558475</t>
   </si>
   <si>
@@ -688,6 +808,9 @@
     <t>PortZacharymouth</t>
   </si>
   <si>
+    <t>74702</t>
+  </si>
+  <si>
     <t>+2524558476</t>
   </si>
   <si>
@@ -709,6 +832,9 @@
     <t>WestWilbur</t>
   </si>
   <si>
+    <t>52324</t>
+  </si>
+  <si>
     <t>+2524558477</t>
   </si>
   <si>
@@ -733,6 +859,9 @@
     <t>PortKendrick</t>
   </si>
   <si>
+    <t>44662</t>
+  </si>
+  <si>
     <t>+2524558478</t>
   </si>
   <si>
@@ -742,7 +871,7 @@
     <t>William</t>
   </si>
   <si>
-    <t>Jully/10/1950</t>
+    <t>July/10/1950</t>
   </si>
   <si>
     <t>870 Somer Place</t>
@@ -757,6 +886,9 @@
     <t>PA</t>
   </si>
   <si>
+    <t>73592</t>
+  </si>
+  <si>
     <t>+2524558479</t>
   </si>
   <si>
@@ -778,6 +910,9 @@
     <t>VT</t>
   </si>
   <si>
+    <t>89215</t>
+  </si>
+  <si>
     <t>+2524558480</t>
   </si>
   <si>
@@ -802,6 +937,9 @@
     <t>Koepphaven</t>
   </si>
   <si>
+    <t>78752</t>
+  </si>
+  <si>
     <t>+2524558481</t>
   </si>
   <si>
@@ -829,6 +967,9 @@
     <t>IA</t>
   </si>
   <si>
+    <t>20862</t>
+  </si>
+  <si>
     <t>+2524558482</t>
   </si>
   <si>
@@ -860,6 +1001,9 @@
   </si>
   <si>
     <t>OH</t>
+  </si>
+  <si>
+    <t>65231</t>
   </si>
   <si>
     <t>+2524558483</t>
@@ -873,9 +1017,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21">
@@ -910,22 +1054,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -939,11 +1083,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -973,21 +1132,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -995,30 +1139,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1032,7 +1153,30 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1059,7 +1203,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1071,79 +1353,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1155,79 +1371,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1294,6 +1438,30 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
@@ -1314,108 +1482,84 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1424,60 +1568,60 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1488,7 +1632,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1505,6 +1649,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1826,12 +1973,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:P32"/>
+  <dimension ref="A1:X32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="149" zoomScaleNormal="149" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="149" zoomScaleNormal="149" topLeftCell="P1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="N31" sqref="N31"/>
+      <selection pane="bottomLeft" activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1852,9 +1999,11 @@
     <col min="14" max="14" width="14" style="1" customWidth="1"/>
     <col min="15" max="15" width="14.375" customWidth="1"/>
     <col min="16" max="16" width="11.75" customWidth="1"/>
+    <col min="20" max="20" width="14.1875" customWidth="1"/>
+    <col min="21" max="21" width="11.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.8" spans="1:16">
+    <row r="1" ht="14.8" spans="1:24">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1903,1399 +2052,2017 @@
       <c r="P1" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>16</v>
+      </c>
+      <c r="X1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" ht="14.8" spans="1:16">
+    <row r="2" ht="14.8" spans="1:24">
       <c r="A2" s="3" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R2">
+        <v>17</v>
+      </c>
+      <c r="S2">
+        <v>2003</v>
+      </c>
+      <c r="T2">
+        <v>8</v>
+      </c>
+      <c r="U2" s="6">
+        <v>37850</v>
+      </c>
+      <c r="V2">
+        <v>18</v>
+      </c>
+      <c r="W2" t="s">
+        <v>39</v>
+      </c>
+      <c r="X2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" ht="14.8" spans="1:24">
+      <c r="A3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2" s="4">
-        <v>19958</v>
-      </c>
-      <c r="N2" s="5" t="s">
+      <c r="C3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="P2" t="s">
-        <v>29</v>
+      <c r="F3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P3" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>53</v>
+      </c>
+      <c r="R3">
+        <v>22</v>
+      </c>
+      <c r="S3">
+        <v>1989</v>
+      </c>
+      <c r="T3">
+        <v>11</v>
+      </c>
+      <c r="U3" s="6">
+        <v>32834</v>
+      </c>
+      <c r="V3">
+        <v>32</v>
+      </c>
+      <c r="W3" t="s">
+        <v>54</v>
+      </c>
+      <c r="X3">
+        <v>2</v>
       </c>
     </row>
-    <row r="3" ht="14.8" spans="1:16">
-      <c r="A3" s="3" t="s">
+    <row r="4" ht="14.8" spans="1:24">
+      <c r="A4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="M3" s="4">
-        <v>48193</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="P3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" ht="14.8" spans="1:16">
-      <c r="A4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="2" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M4" s="4">
-        <v>96884</v>
+        <v>63</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="P4" t="s">
-        <v>53</v>
+        <v>67</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>68</v>
+      </c>
+      <c r="R4">
+        <v>27</v>
+      </c>
+      <c r="S4">
+        <v>1943</v>
+      </c>
+      <c r="T4">
+        <v>6</v>
+      </c>
+      <c r="U4" s="6">
+        <v>15884</v>
+      </c>
+      <c r="V4">
+        <v>79</v>
+      </c>
+      <c r="W4" t="s">
+        <v>69</v>
+      </c>
+      <c r="X4">
+        <v>3</v>
       </c>
     </row>
-    <row r="5" ht="14.8" spans="1:16">
+    <row r="5" ht="14.8" spans="1:24">
       <c r="A5" s="3" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="2" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="M5" s="4">
-        <v>57037</v>
+        <v>76</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="P5" t="s">
-        <v>63</v>
+        <v>80</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>81</v>
+      </c>
+      <c r="R5">
+        <v>7</v>
+      </c>
+      <c r="S5">
+        <v>1991</v>
+      </c>
+      <c r="T5">
+        <v>12</v>
+      </c>
+      <c r="U5" s="6">
+        <v>33579</v>
+      </c>
+      <c r="V5">
+        <v>30</v>
+      </c>
+      <c r="W5" t="s">
+        <v>82</v>
+      </c>
+      <c r="X5">
+        <v>4</v>
       </c>
     </row>
-    <row r="6" ht="14.8" spans="1:16">
+    <row r="6" ht="14.8" spans="1:24">
       <c r="A6" s="3" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M6" s="4">
-        <v>68925</v>
+        <v>90</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>91</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="P6" t="s">
-        <v>73</v>
+        <v>93</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>39</v>
+      </c>
+      <c r="R6">
+        <v>22</v>
+      </c>
+      <c r="S6">
+        <v>1961</v>
+      </c>
+      <c r="T6">
+        <v>1</v>
+      </c>
+      <c r="U6" s="6">
+        <v>22303</v>
+      </c>
+      <c r="V6">
+        <v>61</v>
+      </c>
+      <c r="W6" t="s">
+        <v>94</v>
+      </c>
+      <c r="X6">
+        <v>5</v>
       </c>
     </row>
-    <row r="7" ht="14.8" spans="1:16">
+    <row r="7" ht="14.8" spans="1:24">
       <c r="A7" s="3" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="M7" s="4">
-        <v>88589</v>
+        <v>102</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>103</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="P7" t="s">
-        <v>83</v>
+        <v>105</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>38</v>
+      </c>
+      <c r="R7">
+        <v>31</v>
+      </c>
+      <c r="S7">
+        <v>1971</v>
+      </c>
+      <c r="T7">
+        <v>8</v>
+      </c>
+      <c r="U7" s="6">
+        <v>26176</v>
+      </c>
+      <c r="V7">
+        <v>50</v>
+      </c>
+      <c r="W7" t="s">
+        <v>68</v>
+      </c>
+      <c r="X7">
+        <v>6</v>
       </c>
     </row>
-    <row r="8" ht="14.8" spans="1:16">
+    <row r="8" ht="14.8" spans="1:24">
       <c r="A8" s="3" t="s">
-        <v>84</v>
+        <v>106</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M8" s="4">
-        <v>78519</v>
+        <v>33</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>113</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>91</v>
+        <v>114</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="P8" t="s">
-        <v>92</v>
+        <v>115</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>54</v>
+      </c>
+      <c r="R8">
+        <v>2</v>
+      </c>
+      <c r="S8">
+        <v>1957</v>
+      </c>
+      <c r="T8">
+        <v>2</v>
+      </c>
+      <c r="U8" s="6">
+        <v>20853</v>
+      </c>
+      <c r="V8">
+        <v>65</v>
+      </c>
+      <c r="W8" t="s">
+        <v>116</v>
+      </c>
+      <c r="X8">
+        <v>7</v>
       </c>
     </row>
-    <row r="9" ht="14.8" spans="1:16">
+    <row r="9" ht="14.8" spans="1:24">
       <c r="A9" s="3" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="2" t="s">
-        <v>94</v>
+        <v>118</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>95</v>
+        <v>119</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>96</v>
+        <v>120</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>97</v>
+        <v>121</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>98</v>
+        <v>122</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M9" s="4">
-        <v>30295</v>
+        <v>33</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>124</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
       <c r="P9" t="s">
-        <v>102</v>
+        <v>127</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R9">
+        <v>22</v>
+      </c>
+      <c r="S9">
+        <v>1957</v>
+      </c>
+      <c r="T9">
+        <v>11</v>
+      </c>
+      <c r="U9" s="6">
+        <v>21146</v>
+      </c>
+      <c r="V9">
+        <v>64</v>
+      </c>
+      <c r="W9" t="s">
+        <v>38</v>
+      </c>
+      <c r="X9">
+        <v>8</v>
       </c>
     </row>
-    <row r="10" ht="14.8" spans="1:16">
+    <row r="10" ht="14.8" spans="1:24">
       <c r="A10" s="3" t="s">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>104</v>
+        <v>129</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>105</v>
+        <v>130</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>107</v>
+        <v>132</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2" t="s">
-        <v>108</v>
+        <v>133</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>109</v>
+        <v>134</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="M10" s="4">
-        <v>62931</v>
+        <v>48</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>135</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>110</v>
+        <v>136</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>111</v>
+        <v>137</v>
       </c>
       <c r="P10" t="s">
-        <v>112</v>
+        <v>138</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>81</v>
+      </c>
+      <c r="R10">
+        <v>29</v>
+      </c>
+      <c r="S10">
+        <v>1970</v>
+      </c>
+      <c r="T10">
+        <v>12</v>
+      </c>
+      <c r="U10" s="6">
+        <v>25931</v>
+      </c>
+      <c r="V10">
+        <v>51</v>
+      </c>
+      <c r="W10" t="s">
+        <v>139</v>
+      </c>
+      <c r="X10">
+        <v>9</v>
       </c>
     </row>
-    <row r="11" ht="14.8" spans="1:16">
+    <row r="11" ht="14.8" spans="1:24">
       <c r="A11" s="3" t="s">
-        <v>113</v>
+        <v>140</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="2" t="s">
-        <v>114</v>
+        <v>141</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="P11" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>39</v>
+      </c>
+      <c r="R11">
+        <v>3</v>
+      </c>
+      <c r="S11">
+        <v>1988</v>
+      </c>
+      <c r="T11">
+        <v>1</v>
+      </c>
+      <c r="U11" s="6">
+        <v>32145</v>
+      </c>
+      <c r="V11">
+        <v>34</v>
+      </c>
+      <c r="W11" t="s">
+        <v>152</v>
+      </c>
+      <c r="X11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" ht="14.8" spans="1:24">
+      <c r="A12" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P12" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>39</v>
+      </c>
+      <c r="R12">
         <v>20</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="M11" s="4">
-        <v>39324</v>
-      </c>
-      <c r="N11" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="P11" t="s">
-        <v>123</v>
+      <c r="S12">
+        <v>1986</v>
+      </c>
+      <c r="T12">
+        <v>1</v>
+      </c>
+      <c r="U12" s="6">
+        <v>31432</v>
+      </c>
+      <c r="V12">
+        <v>36</v>
+      </c>
+      <c r="W12" t="s">
+        <v>53</v>
+      </c>
+      <c r="X12">
+        <v>11</v>
       </c>
     </row>
-    <row r="12" ht="14.8" spans="1:16">
-      <c r="A12" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M12" s="4">
-        <v>18672</v>
-      </c>
-      <c r="N12" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="P12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="13" ht="14.8" spans="1:16">
+    <row r="13" ht="14.8" spans="1:24">
       <c r="A13" s="3" t="s">
-        <v>133</v>
+        <v>163</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="2" t="s">
-        <v>134</v>
+        <v>164</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>135</v>
+        <v>165</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>136</v>
+        <v>166</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2" t="s">
-        <v>137</v>
+        <v>167</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>138</v>
+        <v>168</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M13" s="4">
-        <v>82473</v>
+        <v>33</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>169</v>
       </c>
       <c r="N13" s="5" t="s">
-        <v>139</v>
+        <v>170</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="P13" t="s">
-        <v>140</v>
+        <v>171</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>68</v>
+      </c>
+      <c r="R13">
+        <v>4</v>
+      </c>
+      <c r="S13">
+        <v>1971</v>
+      </c>
+      <c r="T13">
+        <v>6</v>
+      </c>
+      <c r="U13" s="6">
+        <v>26088</v>
+      </c>
+      <c r="V13">
+        <v>51</v>
+      </c>
+      <c r="W13" t="s">
+        <v>81</v>
+      </c>
+      <c r="X13">
+        <v>12</v>
       </c>
     </row>
-    <row r="14" ht="14.8" spans="1:16">
+    <row r="14" ht="14.8" spans="1:22">
       <c r="A14" s="3" t="s">
-        <v>141</v>
+        <v>172</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="2" t="s">
-        <v>142</v>
+        <v>173</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>143</v>
+        <v>174</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>144</v>
+        <v>175</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2" t="s">
-        <v>145</v>
+        <v>176</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>146</v>
+        <v>177</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M14" s="4">
-        <v>42626</v>
+        <v>33</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>178</v>
       </c>
       <c r="N14" s="5" t="s">
-        <v>147</v>
+        <v>179</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="P14" t="s">
-        <v>148</v>
+        <v>180</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>69</v>
+      </c>
+      <c r="R14">
+        <v>17</v>
+      </c>
+      <c r="S14">
+        <v>1994</v>
+      </c>
+      <c r="T14">
+        <v>3</v>
+      </c>
+      <c r="U14" s="6">
+        <v>34410</v>
+      </c>
+      <c r="V14">
+        <v>28</v>
       </c>
     </row>
-    <row r="15" ht="14.8" spans="1:16">
+    <row r="15" ht="14.8" spans="1:22">
       <c r="A15" s="3" t="s">
-        <v>149</v>
+        <v>181</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>150</v>
+        <v>182</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>151</v>
+        <v>183</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>152</v>
+        <v>184</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>153</v>
+        <v>185</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2" t="s">
-        <v>154</v>
+        <v>186</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>155</v>
+        <v>187</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M15" s="4">
-        <v>93077</v>
+        <v>33</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>188</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>156</v>
+        <v>189</v>
       </c>
       <c r="O15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P15" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>82</v>
+      </c>
+      <c r="R15">
         <v>28</v>
       </c>
-      <c r="P15" t="s">
-        <v>157</v>
+      <c r="S15">
+        <v>1988</v>
+      </c>
+      <c r="T15">
+        <v>4</v>
+      </c>
+      <c r="U15" s="6">
+        <v>32261</v>
+      </c>
+      <c r="V15">
+        <v>34</v>
       </c>
     </row>
-    <row r="16" ht="14.8" spans="1:16">
+    <row r="16" ht="14.8" spans="1:22">
       <c r="A16" s="3" t="s">
-        <v>158</v>
+        <v>191</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>159</v>
+        <v>192</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>160</v>
+        <v>193</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>161</v>
+        <v>194</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>162</v>
+        <v>195</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2" t="s">
-        <v>163</v>
+        <v>196</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>155</v>
+        <v>187</v>
       </c>
       <c r="L16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="N16" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P16" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q16" t="s">
         <v>38</v>
       </c>
-      <c r="M16" s="4">
-        <v>16820</v>
-      </c>
-      <c r="N16" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="O16" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="P16" t="s">
-        <v>165</v>
+      <c r="R16">
+        <v>31</v>
+      </c>
+      <c r="S16">
+        <v>1979</v>
+      </c>
+      <c r="T16">
+        <v>8</v>
+      </c>
+      <c r="U16" s="6">
+        <v>29098</v>
+      </c>
+      <c r="V16">
+        <v>42</v>
       </c>
     </row>
-    <row r="17" ht="14.8" spans="1:16">
+    <row r="17" ht="14.8" spans="1:22">
       <c r="A17" s="3" t="s">
-        <v>166</v>
+        <v>200</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="2" t="s">
-        <v>167</v>
+        <v>201</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>168</v>
+        <v>202</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>169</v>
+        <v>203</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>170</v>
+        <v>204</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>171</v>
+        <v>205</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>172</v>
+        <v>206</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M17" s="4">
-        <v>32831</v>
+        <v>63</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>207</v>
       </c>
       <c r="N17" s="5" t="s">
-        <v>173</v>
+        <v>208</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="P17" t="s">
-        <v>174</v>
+        <v>209</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>81</v>
+      </c>
+      <c r="R17">
+        <v>8</v>
+      </c>
+      <c r="S17">
+        <v>1972</v>
+      </c>
+      <c r="T17">
+        <v>12</v>
+      </c>
+      <c r="U17" s="6">
+        <v>26641</v>
+      </c>
+      <c r="V17">
+        <v>49</v>
       </c>
     </row>
-    <row r="18" ht="14.8" spans="1:16">
+    <row r="18" ht="14.8" spans="1:22">
       <c r="A18" s="3" t="s">
-        <v>175</v>
+        <v>210</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>176</v>
+        <v>211</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>177</v>
+        <v>212</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>178</v>
+        <v>213</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>179</v>
+        <v>214</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>180</v>
+        <v>215</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>181</v>
+        <v>216</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>182</v>
+        <v>217</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="M18" s="4">
-        <v>18661</v>
+        <v>76</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>218</v>
       </c>
       <c r="N18" s="5" t="s">
-        <v>183</v>
+        <v>219</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="P18" t="s">
-        <v>184</v>
+        <v>220</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>81</v>
+      </c>
+      <c r="R18">
+        <v>10</v>
+      </c>
+      <c r="S18">
+        <v>1935</v>
+      </c>
+      <c r="T18">
+        <v>12</v>
+      </c>
+      <c r="U18" s="6">
+        <v>13128</v>
+      </c>
+      <c r="V18">
+        <v>86</v>
       </c>
     </row>
-    <row r="19" ht="14.8" spans="1:16">
+    <row r="19" ht="14.8" spans="1:22">
       <c r="A19" s="3" t="s">
-        <v>185</v>
+        <v>221</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="2" t="s">
-        <v>186</v>
+        <v>222</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>187</v>
+        <v>223</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>188</v>
+        <v>224</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2" t="s">
-        <v>189</v>
+        <v>225</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>190</v>
+        <v>226</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M19" s="4">
-        <v>57502</v>
+        <v>90</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>227</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>191</v>
+        <v>228</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="P19" t="s">
-        <v>192</v>
+        <v>229</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>53</v>
+      </c>
+      <c r="R19">
+        <v>3</v>
+      </c>
+      <c r="S19">
+        <v>1948</v>
+      </c>
+      <c r="T19">
+        <v>11</v>
+      </c>
+      <c r="U19" s="6">
+        <v>17840</v>
+      </c>
+      <c r="V19">
+        <v>73</v>
       </c>
     </row>
-    <row r="20" ht="14.8" spans="1:16">
+    <row r="20" ht="14.8" spans="1:22">
       <c r="A20" s="3" t="s">
-        <v>193</v>
+        <v>230</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="2" t="s">
-        <v>194</v>
+        <v>231</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>195</v>
+        <v>232</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>196</v>
+        <v>233</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>197</v>
+        <v>234</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>198</v>
+        <v>235</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="M20" s="4">
-        <v>44872</v>
+        <v>102</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>236</v>
       </c>
       <c r="N20" s="5" t="s">
-        <v>199</v>
+        <v>237</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="P20" t="s">
-        <v>200</v>
+        <v>238</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>68</v>
+      </c>
+      <c r="R20">
+        <v>27</v>
+      </c>
+      <c r="S20">
+        <v>1926</v>
+      </c>
+      <c r="T20">
+        <v>6</v>
+      </c>
+      <c r="U20" s="6">
+        <v>9675</v>
+      </c>
+      <c r="V20">
+        <v>96</v>
       </c>
     </row>
-    <row r="21" ht="14.8" spans="1:16">
+    <row r="21" ht="14.8" spans="1:22">
       <c r="A21" s="3" t="s">
-        <v>201</v>
+        <v>239</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="2" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>202</v>
+        <v>240</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>203</v>
+        <v>241</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>204</v>
+        <v>242</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>205</v>
+        <v>243</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>206</v>
+        <v>244</v>
       </c>
       <c r="L21" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="N21" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="P21" t="s">
+        <v>247</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>116</v>
+      </c>
+      <c r="R21">
         <v>26</v>
       </c>
-      <c r="M21" s="4">
-        <v>81932</v>
-      </c>
-      <c r="N21" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="O21" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="P21" t="s">
-        <v>208</v>
+      <c r="S21">
+        <v>1960</v>
+      </c>
+      <c r="T21">
+        <v>7</v>
+      </c>
+      <c r="U21" s="6">
+        <v>22123</v>
+      </c>
+      <c r="V21">
+        <v>61</v>
       </c>
     </row>
-    <row r="22" ht="14.8" spans="1:16">
+    <row r="22" ht="14.8" spans="1:22">
       <c r="A22" s="3" t="s">
-        <v>209</v>
+        <v>248</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>210</v>
+        <v>249</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>211</v>
+        <v>250</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>212</v>
+        <v>251</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>213</v>
+        <v>252</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>214</v>
+        <v>253</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>215</v>
+        <v>254</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>206</v>
+        <v>244</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M22" s="4">
-        <v>77790</v>
+        <v>33</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>255</v>
       </c>
       <c r="N22" s="5" t="s">
-        <v>216</v>
+        <v>256</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="P22" t="s">
-        <v>217</v>
+        <v>257</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>116</v>
+      </c>
+      <c r="R22">
+        <v>8</v>
+      </c>
+      <c r="S22">
+        <v>1937</v>
+      </c>
+      <c r="T22">
+        <v>7</v>
+      </c>
+      <c r="U22" s="6">
+        <v>13704</v>
+      </c>
+      <c r="V22">
+        <v>84</v>
       </c>
     </row>
-    <row r="23" ht="14.8" spans="1:16">
+    <row r="23" ht="14.8" spans="1:22">
       <c r="A23" s="3" t="s">
-        <v>218</v>
+        <v>258</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>219</v>
+        <v>259</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>220</v>
+        <v>260</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>221</v>
+        <v>261</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>222</v>
+        <v>262</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>146</v>
+        <v>177</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="M23" s="4">
-        <v>74702</v>
+        <v>48</v>
+      </c>
+      <c r="M23" s="4" t="s">
+        <v>264</v>
       </c>
       <c r="N23" s="5" t="s">
-        <v>224</v>
+        <v>265</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="P23" t="s">
-        <v>225</v>
+        <v>266</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>39</v>
+      </c>
+      <c r="R23">
+        <v>25</v>
+      </c>
+      <c r="S23">
+        <v>1963</v>
+      </c>
+      <c r="T23">
+        <v>1</v>
+      </c>
+      <c r="U23" s="6">
+        <v>23036</v>
+      </c>
+      <c r="V23">
+        <v>59</v>
       </c>
     </row>
-    <row r="24" ht="14.8" spans="1:16">
+    <row r="24" ht="14.8" spans="1:22">
       <c r="A24" s="3" t="s">
-        <v>226</v>
+        <v>267</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="2" t="s">
-        <v>227</v>
+        <v>268</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>228</v>
+        <v>269</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>229</v>
+        <v>270</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2" t="s">
-        <v>230</v>
+        <v>271</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="M24" s="4">
-        <v>52324</v>
+        <v>147</v>
+      </c>
+      <c r="M24" s="4" t="s">
+        <v>272</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>231</v>
+        <v>273</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>122</v>
+        <v>150</v>
       </c>
       <c r="P24" t="s">
-        <v>232</v>
+        <v>274</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>139</v>
+      </c>
+      <c r="R24">
+        <v>29</v>
+      </c>
+      <c r="S24">
+        <v>1974</v>
+      </c>
+      <c r="T24">
+        <v>9</v>
+      </c>
+      <c r="U24" s="6">
+        <v>27301</v>
+      </c>
+      <c r="V24">
+        <v>47</v>
       </c>
     </row>
-    <row r="25" ht="14.8" spans="1:16">
+    <row r="25" ht="14.8" spans="1:22">
       <c r="A25" s="3" t="s">
-        <v>233</v>
+        <v>275</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>94</v>
+        <v>118</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>234</v>
+        <v>276</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>235</v>
+        <v>277</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>236</v>
+        <v>278</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>237</v>
+        <v>279</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>238</v>
+        <v>280</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>155</v>
+        <v>187</v>
       </c>
       <c r="L25" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M25" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="N25" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P25" t="s">
+        <v>283</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>39</v>
+      </c>
+      <c r="R25">
         <v>26</v>
       </c>
-      <c r="M25" s="4">
-        <v>44662</v>
-      </c>
-      <c r="N25" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="O25" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="P25" t="s">
-        <v>240</v>
+      <c r="S25">
+        <v>1962</v>
+      </c>
+      <c r="T25">
+        <v>1</v>
+      </c>
+      <c r="U25" s="6">
+        <v>22672</v>
+      </c>
+      <c r="V25">
+        <v>60</v>
       </c>
     </row>
-    <row r="26" ht="14.8" spans="1:16">
+    <row r="26" ht="14.8" spans="1:22">
       <c r="A26" s="3" t="s">
-        <v>241</v>
+        <v>284</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="2" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>242</v>
+        <v>285</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>243</v>
+        <v>286</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>244</v>
+        <v>287</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>245</v>
+        <v>288</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>246</v>
+        <v>289</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M26" s="4">
-        <v>73592</v>
+        <v>33</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>290</v>
       </c>
       <c r="N26" s="5" t="s">
-        <v>247</v>
+        <v>291</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="P26" t="s">
-        <v>248</v>
+        <v>292</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>116</v>
+      </c>
+      <c r="R26">
+        <v>10</v>
+      </c>
+      <c r="S26">
+        <v>1950</v>
+      </c>
+      <c r="T26">
+        <v>7</v>
+      </c>
+      <c r="U26" s="6">
+        <v>18454</v>
+      </c>
+      <c r="V26">
+        <v>71</v>
       </c>
     </row>
-    <row r="27" ht="14.8" spans="1:16">
+    <row r="27" ht="14.8" spans="1:22">
       <c r="A27" s="3" t="s">
-        <v>249</v>
+        <v>293</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="2" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>250</v>
+        <v>294</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>251</v>
+        <v>295</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="2" t="s">
-        <v>252</v>
+        <v>296</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>253</v>
+        <v>297</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M27" s="4">
-        <v>89215</v>
+        <v>33</v>
+      </c>
+      <c r="M27" s="4" t="s">
+        <v>298</v>
       </c>
       <c r="N27" s="5" t="s">
-        <v>254</v>
+        <v>299</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="P27" t="s">
-        <v>255</v>
+        <v>300</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>82</v>
+      </c>
+      <c r="R27">
+        <v>23</v>
+      </c>
+      <c r="S27">
+        <v>1969</v>
+      </c>
+      <c r="T27">
+        <v>4</v>
+      </c>
+      <c r="U27" s="6">
+        <v>25316</v>
+      </c>
+      <c r="V27">
+        <v>53</v>
       </c>
     </row>
-    <row r="28" ht="14.8" spans="1:16">
+    <row r="28" ht="14.8" spans="1:22">
       <c r="A28" s="3" t="s">
-        <v>256</v>
+        <v>301</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>257</v>
+        <v>302</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>258</v>
+        <v>303</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>259</v>
+        <v>304</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>260</v>
+        <v>305</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="2" t="s">
-        <v>261</v>
+        <v>306</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>146</v>
+        <v>177</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M28" s="4">
-        <v>78752</v>
+        <v>33</v>
+      </c>
+      <c r="M28" s="4" t="s">
+        <v>307</v>
       </c>
       <c r="N28" s="5" t="s">
-        <v>262</v>
+        <v>308</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="P28" t="s">
-        <v>263</v>
+        <v>309</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>81</v>
+      </c>
+      <c r="R28">
+        <v>12</v>
+      </c>
+      <c r="S28">
+        <v>1978</v>
+      </c>
+      <c r="T28">
+        <v>12</v>
+      </c>
+      <c r="U28" s="6">
+        <v>28836</v>
+      </c>
+      <c r="V28">
+        <v>43</v>
       </c>
     </row>
-    <row r="29" ht="14.8" spans="1:16">
+    <row r="29" ht="14.8" spans="1:22">
       <c r="A29" s="3" t="s">
-        <v>264</v>
+        <v>310</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="2" t="s">
-        <v>265</v>
+        <v>311</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>266</v>
+        <v>312</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>267</v>
+        <v>313</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>268</v>
+        <v>314</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>269</v>
+        <v>315</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>270</v>
+        <v>316</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M29" s="4">
-        <v>20862</v>
+        <v>33</v>
+      </c>
+      <c r="M29" s="4" t="s">
+        <v>317</v>
       </c>
       <c r="N29" s="5" t="s">
-        <v>271</v>
+        <v>318</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>272</v>
+        <v>319</v>
       </c>
       <c r="P29" t="s">
-        <v>273</v>
+        <v>320</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>68</v>
+      </c>
+      <c r="R29">
+        <v>25</v>
+      </c>
+      <c r="S29">
+        <v>1972</v>
+      </c>
+      <c r="T29">
+        <v>6</v>
+      </c>
+      <c r="U29" s="6">
+        <v>26475</v>
+      </c>
+      <c r="V29">
+        <v>49</v>
       </c>
     </row>
-    <row r="30" ht="14.8" spans="1:16">
+    <row r="30" ht="14.8" spans="1:22">
       <c r="A30" s="3" t="s">
-        <v>274</v>
+        <v>321</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>275</v>
+        <v>322</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>276</v>
+        <v>323</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>277</v>
+        <v>324</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>278</v>
+        <v>325</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>279</v>
+        <v>326</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>280</v>
+        <v>327</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>281</v>
+        <v>328</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M30" s="4">
-        <v>65231</v>
+        <v>33</v>
+      </c>
+      <c r="M30" s="4" t="s">
+        <v>329</v>
       </c>
       <c r="N30" s="5" t="s">
-        <v>282</v>
+        <v>330</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>122</v>
+        <v>150</v>
       </c>
       <c r="P30" t="s">
-        <v>283</v>
+        <v>331</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>139</v>
+      </c>
+      <c r="R30">
+        <v>16</v>
+      </c>
+      <c r="S30">
+        <v>1998</v>
+      </c>
+      <c r="T30">
+        <v>9</v>
+      </c>
+      <c r="U30" s="6">
+        <v>36054</v>
+      </c>
+      <c r="V30">
+        <v>23</v>
       </c>
     </row>
     <row r="31" ht="14.8" spans="1:15">

</xml_diff>